<commit_message>
Se deja funcional todo el modulo de ubicaciones y movimientos y se relaciona con el de inventario
</commit_message>
<xml_diff>
--- a/tests/prueba_productos.xlsx
+++ b/tests/prueba_productos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\ProyectoAnalisis\Sistema de inventariado\TotalStock\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EA9E1E-04B8-4545-A482-C3037CEB1471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3164D325-1526-4CBA-9EFE-7B94DEE2E88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="1480" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Nombre</t>
   </si>
   <si>
     <t>Precio</t>
-  </si>
-  <si>
-    <t>Cantidad</t>
   </si>
   <si>
     <t>Cadena</t>
@@ -125,14 +122,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2302EF9A-54F7-415C-82F9-A018CC83447B}" name="Tabla1" displayName="Tabla1" ref="A1:E6" totalsRowShown="0">
-  <autoFilter ref="A1:E6" xr:uid="{2302EF9A-54F7-415C-82F9-A018CC83447B}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2302EF9A-54F7-415C-82F9-A018CC83447B}" name="Tabla1" displayName="Tabla1" ref="A1:D6" totalsRowShown="0">
+  <autoFilter ref="A1:D6" xr:uid="{2302EF9A-54F7-415C-82F9-A018CC83447B}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D9890C4A-8D1D-4570-9E23-C773AFBFBE43}" name="Modelo"/>
     <tableColumn id="5" xr3:uid="{D46793FF-F99E-41CD-B2ED-49B7FD306E45}" name="Tipo"/>
     <tableColumn id="2" xr3:uid="{0D94AD97-E7C8-4626-A422-731A9BE8DB31}" name="Nombre"/>
     <tableColumn id="3" xr3:uid="{09A36FB0-72CE-49AE-996B-89D542A53B78}" name="Precio"/>
-    <tableColumn id="4" xr3:uid="{DAA7FD20-0B9A-49F0-96C2-435A146A925F}" name="Cantidad"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -401,23 +397,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="11.26953125" customWidth="1"/>
+    <col min="1" max="4" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -425,97 +421,80 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1234</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>400</v>
-      </c>
-      <c r="E2">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>123</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>35</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+        <v>365</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>324</v>
       </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5432</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>856</v>
       </c>
-      <c r="E5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>543</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>55</v>
       </c>
-      <c r="E6">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G8" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>